<commit_message>
dejo terminado el conversor de ficheros excel para el TPV con Panda, comentado lo hecho con openpyxl
</commit_message>
<xml_diff>
--- a/app/datos/tarifas_a_TPV/export_sqlpyme.xlsx
+++ b/app/datos/tarifas_a_TPV/export_sqlpyme.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nube\GitHub\Mallorquina_API\app\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Mallorquina_API\app\datos\tarifas_a_TPV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA60132-50AD-45D2-AC42-C41023604310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC70F42C-AE89-44D7-BCF4-0B85BB2F4AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3800" windowWidth="38470" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="13372" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sql a tpv" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="32">
   <si>
     <t>Código</t>
   </si>
@@ -101,6 +101,21 @@
   </si>
   <si>
     <t>dddd</t>
+  </si>
+  <si>
+    <t>12.34</t>
+  </si>
+  <si>
+    <t>13.1</t>
+  </si>
+  <si>
+    <t>22.4</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>1.2</t>
   </si>
 </sst>
 </file>
@@ -473,33 +488,33 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.07421875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.53515625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.54296875" style="1"/>
+    <col min="15" max="15" width="18.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.53515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -555,7 +570,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -572,7 +587,7 @@
         <v>45636</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>21</v>
@@ -587,7 +602,7 @@
         <v>23</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>23</v>
@@ -611,7 +626,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -628,7 +643,7 @@
         <v>45636</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>21</v>
@@ -646,7 +661,7 @@
         <v>23</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>23</v>
@@ -661,7 +676,7 @@
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -680,23 +695,21 @@
       <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>23</v>
@@ -711,7 +724,7 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
     </row>
-    <row r="5" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -734,7 +747,7 @@
         <v>21</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>23</v>
@@ -761,7 +774,7 @@
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
     </row>
-    <row r="6" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -783,11 +796,9 @@
       <c r="G6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>23</v>
@@ -811,7 +822,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
     </row>
-    <row r="7" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>

</xml_diff>